<commit_message>
Construccion de rutas para operaciones CRUD
</commit_message>
<xml_diff>
--- a/Documentación/PRODUCT_BACKLOG.xlsx
+++ b/Documentación/PRODUCT_BACKLOG.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jahel Nogales\git\RankingBank\Documentación\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E818773-A74E-42A9-8947-5D19C77A0B44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AB0C9DC-E4A7-4DC6-85C7-4A8FF3C33420}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{CCBAC7FC-6E9C-4FC6-B199-5A9E8318DAC7}"/>
+    <workbookView xWindow="1560" yWindow="1080" windowWidth="14370" windowHeight="15120" xr2:uid="{CCBAC7FC-6E9C-4FC6-B199-5A9E8318DAC7}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="89">
   <si>
     <t>PRODUCT BACKLOG</t>
   </si>
@@ -295,16 +295,16 @@
     <t>RQ-08</t>
   </si>
   <si>
-    <t>microcréditos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Como administrador requiero que los asesores de microcréditos puedan  iniciar sesión en la aplicación </t>
-  </si>
-  <si>
     <t>Como administrador requiero establecer la meta mensual  para los asesores de microcréditos.</t>
   </si>
   <si>
     <t>Como administrador, requiero que se  visualice el ranking de los asesores de microcréditos en tiempo real.</t>
+  </si>
+  <si>
+    <t>Como asesor de microcrédito requiero ingresar la información de los microcréditos otorgados.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Como administrador requiero que los asesores de microcréditos y supervisores puedan  iniciar sesión en la aplicación </t>
   </si>
 </sst>
 </file>
@@ -481,7 +481,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -531,21 +531,6 @@
       </right>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thick">
-        <color theme="4"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -691,9 +676,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -711,10 +693,10 @@
     <xf numFmtId="0" fontId="15" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -741,22 +723,25 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1091,7 +1076,7 @@
   <dimension ref="A1:M31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="105" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1140,17 +1125,17 @@
       <c r="K2" s="44"/>
     </row>
     <row r="3" spans="1:13" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="28"/>
-      <c r="B3" s="28"/>
-      <c r="C3" s="28"/>
-      <c r="D3" s="28"/>
-      <c r="E3" s="28"/>
-      <c r="F3" s="28"/>
-      <c r="G3" s="28"/>
-      <c r="H3" s="28"/>
-      <c r="I3" s="28"/>
-      <c r="J3" s="28"/>
-      <c r="K3" s="28"/>
+      <c r="A3" s="27"/>
+      <c r="B3" s="27"/>
+      <c r="C3" s="27"/>
+      <c r="D3" s="27"/>
+      <c r="E3" s="27"/>
+      <c r="F3" s="27"/>
+      <c r="G3" s="27"/>
+      <c r="H3" s="27"/>
+      <c r="I3" s="27"/>
+      <c r="J3" s="27"/>
+      <c r="K3" s="27"/>
     </row>
     <row r="4" spans="1:13" s="15" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="42" t="s">
@@ -1168,53 +1153,53 @@
       <c r="K4" s="42"/>
     </row>
     <row r="5" spans="1:13" ht="42.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="21" t="s">
+      <c r="A5" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="21" t="s">
+      <c r="B5" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="21" t="s">
+      <c r="C5" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="21" t="s">
+      <c r="D5" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="E5" s="22" t="s">
+      <c r="E5" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="F5" s="22" t="s">
+      <c r="F5" s="21" t="s">
         <v>79</v>
       </c>
-      <c r="G5" s="21" t="s">
+      <c r="G5" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="H5" s="24" t="s">
+      <c r="H5" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="I5" s="23" t="s">
+      <c r="I5" s="22" t="s">
         <v>54</v>
       </c>
-      <c r="J5" s="23" t="s">
+      <c r="J5" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="K5" s="25" t="s">
+      <c r="K5" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="L5" s="27"/>
-      <c r="M5" s="26"/>
-    </row>
-    <row r="6" spans="1:13" ht="29.25" x14ac:dyDescent="0.25">
+      <c r="L5" s="26"/>
+      <c r="M5" s="25"/>
+    </row>
+    <row r="6" spans="1:13" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="C6" s="29" t="s">
+        <v>88</v>
+      </c>
+      <c r="C6" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="D6" s="30"/>
+      <c r="D6" s="29"/>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
       <c r="G6" s="4"/>
@@ -1238,10 +1223,10 @@
       <c r="B7" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="29" t="s">
+      <c r="C7" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="D7" s="30"/>
+      <c r="D7" s="29"/>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
@@ -1251,34 +1236,34 @@
       <c r="I7" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="J7" s="32" t="s">
+      <c r="J7" s="31" t="s">
         <v>63</v>
       </c>
       <c r="K7" s="4" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" ht="29.25" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="C8" s="29" t="s">
+        <v>87</v>
+      </c>
+      <c r="C8" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="D8" s="30"/>
+      <c r="D8" s="29"/>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
       <c r="H8" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="I8" s="32" t="s">
+      <c r="I8" s="31" t="s">
         <v>58</v>
       </c>
-      <c r="J8" s="33" t="s">
+      <c r="J8" s="32" t="s">
         <v>59</v>
       </c>
       <c r="K8" s="4" t="s">
@@ -1292,10 +1277,10 @@
       <c r="B9" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C9" s="29" t="s">
+      <c r="C9" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="D9" s="30"/>
+      <c r="D9" s="29"/>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
       <c r="G9" s="4"/>
@@ -1305,7 +1290,7 @@
       <c r="I9" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="J9" s="34" t="s">
+      <c r="J9" s="33" t="s">
         <v>61</v>
       </c>
       <c r="K9" s="4" t="s">
@@ -1319,10 +1304,10 @@
       <c r="B10" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="29" t="s">
+      <c r="C10" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="D10" s="30"/>
+      <c r="D10" s="29"/>
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
       <c r="G10" s="4"/>
@@ -1332,7 +1317,7 @@
       <c r="I10" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="J10" s="32" t="s">
+      <c r="J10" s="31" t="s">
         <v>62</v>
       </c>
       <c r="K10" s="4" t="s">
@@ -1344,12 +1329,12 @@
         <v>12</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="C11" s="29" t="s">
+        <v>85</v>
+      </c>
+      <c r="C11" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="D11" s="30"/>
+      <c r="D11" s="29"/>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
       <c r="G11" s="4"/>
@@ -1359,7 +1344,7 @@
       <c r="I11" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="J11" s="32" t="s">
+      <c r="J11" s="31" t="s">
         <v>65</v>
       </c>
       <c r="K11" s="4" t="s">
@@ -1371,12 +1356,12 @@
         <v>27</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="C12" s="29" t="s">
+        <v>86</v>
+      </c>
+      <c r="C12" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="D12" s="30"/>
+      <c r="D12" s="29"/>
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
       <c r="G12" s="4"/>
@@ -1386,7 +1371,7 @@
       <c r="I12" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="J12" s="32" t="s">
+      <c r="J12" s="31" t="s">
         <v>66</v>
       </c>
       <c r="K12" s="4" t="s">
@@ -1400,10 +1385,10 @@
       <c r="B13" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="C13" s="29" t="s">
+      <c r="C13" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="D13" s="30"/>
+      <c r="D13" s="29"/>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
@@ -1413,7 +1398,7 @@
       <c r="I13" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="J13" s="32" t="s">
+      <c r="J13" s="31" t="s">
         <v>83</v>
       </c>
       <c r="K13" s="4" t="s">
@@ -1429,11 +1414,11 @@
       <c r="F14" s="8"/>
       <c r="G14" s="8"/>
       <c r="H14" s="8"/>
-      <c r="I14" s="35"/>
-      <c r="J14" s="35"/>
+      <c r="I14" s="34"/>
+      <c r="J14" s="34"/>
       <c r="K14" s="8"/>
     </row>
-    <row r="15" spans="1:13" s="15" customFormat="1" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" s="15" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="42" t="s">
         <v>23</v>
       </c>
@@ -1448,7 +1433,7 @@
       <c r="J15" s="42"/>
       <c r="K15" s="42"/>
     </row>
-    <row r="16" spans="1:13" ht="29.25" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
         <v>13</v>
       </c>
@@ -1458,7 +1443,7 @@
       <c r="C16" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="D16" s="16" t="s">
+      <c r="D16" s="39" t="s">
         <v>38</v>
       </c>
       <c r="E16" s="4">
@@ -1476,7 +1461,7 @@
       <c r="I16" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="J16" s="31"/>
+      <c r="J16" s="30"/>
       <c r="K16" s="4"/>
     </row>
     <row r="17" spans="1:11" ht="28.5" x14ac:dyDescent="0.25">
@@ -1486,20 +1471,28 @@
       <c r="B17" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="C17" s="29" t="s">
-        <v>36</v>
-      </c>
-      <c r="D17" s="30"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
+      <c r="C17" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="D17" s="39" t="s">
+        <v>38</v>
+      </c>
+      <c r="E17" s="4">
+        <v>12</v>
+      </c>
+      <c r="F17" s="4">
+        <v>12</v>
+      </c>
+      <c r="G17" s="4">
+        <v>2</v>
+      </c>
       <c r="H17" s="4" t="s">
         <v>22</v>
       </c>
       <c r="I17" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="J17" s="31"/>
+      <c r="J17" s="30"/>
       <c r="K17" s="4"/>
     </row>
     <row r="18" spans="1:11" ht="29.25" x14ac:dyDescent="0.25">
@@ -1509,20 +1502,28 @@
       <c r="B18" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C18" s="29" t="s">
+      <c r="C18" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="D18" s="30"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
-      <c r="G18" s="4"/>
+      <c r="D18" s="29" t="s">
+        <v>51</v>
+      </c>
+      <c r="E18" s="4">
+        <v>40</v>
+      </c>
+      <c r="F18" s="4">
+        <v>25</v>
+      </c>
+      <c r="G18" s="4">
+        <v>2</v>
+      </c>
       <c r="H18" s="4" t="s">
         <v>22</v>
       </c>
       <c r="I18" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="J18" s="31"/>
+      <c r="J18" s="30"/>
       <c r="K18" s="4"/>
     </row>
     <row r="19" spans="1:11" ht="29.25" x14ac:dyDescent="0.25">
@@ -1532,10 +1533,10 @@
       <c r="B19" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C19" s="29" t="s">
+      <c r="C19" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="D19" s="30"/>
+      <c r="D19" s="29"/>
       <c r="E19" s="4"/>
       <c r="F19" s="4"/>
       <c r="G19" s="4"/>
@@ -1545,7 +1546,7 @@
       <c r="I19" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="J19" s="31"/>
+      <c r="J19" s="30"/>
       <c r="K19" s="4"/>
     </row>
     <row r="20" spans="1:11" ht="28.5" x14ac:dyDescent="0.25">
@@ -1555,10 +1556,10 @@
       <c r="B20" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="C20" s="29" t="s">
+      <c r="C20" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="D20" s="30"/>
+      <c r="D20" s="29"/>
       <c r="E20" s="4"/>
       <c r="F20" s="4"/>
       <c r="G20" s="4"/>
@@ -1568,7 +1569,7 @@
       <c r="I20" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="J20" s="31"/>
+      <c r="J20" s="30"/>
       <c r="K20" s="4"/>
     </row>
     <row r="21" spans="1:11" ht="28.5" x14ac:dyDescent="0.25">
@@ -1578,10 +1579,10 @@
       <c r="B21" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="C21" s="29" t="s">
+      <c r="C21" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="D21" s="30"/>
+      <c r="D21" s="29"/>
       <c r="E21" s="4"/>
       <c r="F21" s="4"/>
       <c r="G21" s="4"/>
@@ -1591,7 +1592,7 @@
       <c r="I21" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="J21" s="31"/>
+      <c r="J21" s="30"/>
       <c r="K21" s="4"/>
     </row>
     <row r="22" spans="1:11" ht="28.5" x14ac:dyDescent="0.25">
@@ -1601,10 +1602,10 @@
       <c r="B22" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="C22" s="29" t="s">
+      <c r="C22" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="D22" s="30"/>
+      <c r="D22" s="29"/>
       <c r="E22" s="4"/>
       <c r="F22" s="4"/>
       <c r="G22" s="4"/>
@@ -1614,38 +1615,38 @@
       <c r="I22" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="J22" s="31"/>
+      <c r="J22" s="30"/>
       <c r="K22" s="4"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="35"/>
-      <c r="B23" s="35"/>
+      <c r="A23" s="34"/>
+      <c r="B23" s="34"/>
       <c r="C23" s="8"/>
       <c r="D23" s="8"/>
       <c r="E23" s="8"/>
       <c r="F23" s="8"/>
       <c r="G23" s="8"/>
       <c r="H23" s="8"/>
-      <c r="I23" s="35"/>
-      <c r="J23" s="35"/>
+      <c r="I23" s="34"/>
+      <c r="J23" s="34"/>
       <c r="K23" s="8"/>
     </row>
     <row r="24" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="35"/>
-      <c r="B24" s="35"/>
+      <c r="A24" s="34"/>
+      <c r="B24" s="34"/>
       <c r="C24" s="8"/>
       <c r="D24" s="8"/>
       <c r="E24" s="8"/>
       <c r="F24" s="8"/>
       <c r="G24" s="8"/>
       <c r="H24" s="8"/>
-      <c r="I24" s="35"/>
-      <c r="J24" s="35"/>
+      <c r="I24" s="34"/>
+      <c r="J24" s="34"/>
       <c r="K24" s="8"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="35"/>
-      <c r="B25" s="35"/>
+      <c r="A25" s="34"/>
+      <c r="B25" s="34"/>
       <c r="C25" s="8"/>
       <c r="D25" s="8"/>
       <c r="E25" s="40" t="s">
@@ -1656,116 +1657,116 @@
         <v>77</v>
       </c>
       <c r="H25" s="41"/>
-      <c r="I25" s="35"/>
-      <c r="J25" s="35"/>
+      <c r="I25" s="34"/>
+      <c r="J25" s="34"/>
       <c r="K25" s="8"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="35"/>
-      <c r="B26" s="35"/>
+      <c r="A26" s="34"/>
+      <c r="B26" s="34"/>
       <c r="C26" s="8"/>
       <c r="D26" s="8"/>
-      <c r="E26" s="36" t="s">
+      <c r="E26" s="35" t="s">
         <v>73</v>
       </c>
-      <c r="F26" s="37">
+      <c r="F26" s="36">
         <f>SUM(E6:E12)+SUM(E16:E22)</f>
-        <v>12</v>
-      </c>
-      <c r="G26" s="36" t="s">
+        <v>64</v>
+      </c>
+      <c r="G26" s="35" t="s">
         <v>73</v>
       </c>
-      <c r="H26" s="37">
+      <c r="H26" s="36">
         <f>SUM(F6:F12)+SUM(F16:F22)</f>
-        <v>12</v>
-      </c>
-      <c r="I26" s="35"/>
-      <c r="J26" s="35"/>
+        <v>49</v>
+      </c>
+      <c r="I26" s="34"/>
+      <c r="J26" s="34"/>
       <c r="K26" s="8"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="35"/>
-      <c r="B27" s="35"/>
+      <c r="A27" s="34"/>
+      <c r="B27" s="34"/>
       <c r="C27" s="8"/>
       <c r="D27" s="8"/>
-      <c r="E27" s="36" t="s">
+      <c r="E27" s="35" t="s">
         <v>74</v>
       </c>
-      <c r="F27" s="37">
+      <c r="F27" s="36">
         <f>F26/24</f>
-        <v>0.5</v>
-      </c>
-      <c r="G27" s="36" t="s">
+        <v>2.6666666666666665</v>
+      </c>
+      <c r="G27" s="35" t="s">
         <v>74</v>
       </c>
-      <c r="H27" s="37">
+      <c r="H27" s="36">
         <f>H26/24</f>
-        <v>0.5</v>
-      </c>
-      <c r="I27" s="35"/>
-      <c r="J27" s="35"/>
+        <v>2.0416666666666665</v>
+      </c>
+      <c r="I27" s="34"/>
+      <c r="J27" s="34"/>
       <c r="K27" s="8"/>
     </row>
     <row r="28" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="35"/>
-      <c r="B28" s="35"/>
+      <c r="A28" s="34"/>
+      <c r="B28" s="34"/>
       <c r="C28" s="8"/>
       <c r="D28" s="8"/>
-      <c r="E28" s="38" t="s">
+      <c r="E28" s="37" t="s">
         <v>75</v>
       </c>
-      <c r="F28" s="39">
+      <c r="F28" s="38">
         <f>F27/7</f>
-        <v>7.1428571428571425E-2</v>
-      </c>
-      <c r="G28" s="38" t="s">
+        <v>0.38095238095238093</v>
+      </c>
+      <c r="G28" s="37" t="s">
         <v>75</v>
       </c>
-      <c r="H28" s="39">
+      <c r="H28" s="38">
         <f>H27/7</f>
-        <v>7.1428571428571425E-2</v>
-      </c>
-      <c r="I28" s="35"/>
-      <c r="J28" s="35"/>
+        <v>0.29166666666666663</v>
+      </c>
+      <c r="I28" s="34"/>
+      <c r="J28" s="34"/>
       <c r="K28" s="8"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="35"/>
-      <c r="B29" s="35"/>
+      <c r="A29" s="34"/>
+      <c r="B29" s="34"/>
       <c r="C29" s="8"/>
       <c r="D29" s="8"/>
       <c r="E29" s="8"/>
       <c r="F29" s="8"/>
       <c r="G29" s="8"/>
       <c r="H29" s="8"/>
-      <c r="I29" s="35"/>
-      <c r="J29" s="35"/>
+      <c r="I29" s="34"/>
+      <c r="J29" s="34"/>
       <c r="K29" s="8"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="35"/>
-      <c r="B30" s="35"/>
+      <c r="A30" s="34"/>
+      <c r="B30" s="34"/>
       <c r="C30" s="8"/>
       <c r="D30" s="8"/>
       <c r="E30" s="8"/>
       <c r="F30" s="8"/>
       <c r="G30" s="8"/>
       <c r="H30" s="8"/>
-      <c r="I30" s="35"/>
-      <c r="J30" s="35"/>
+      <c r="I30" s="34"/>
+      <c r="J30" s="34"/>
       <c r="K30" s="8"/>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" s="35"/>
-      <c r="B31" s="35"/>
+      <c r="A31" s="34"/>
+      <c r="B31" s="34"/>
       <c r="C31" s="8"/>
       <c r="D31" s="8"/>
       <c r="E31" s="8"/>
       <c r="F31" s="8"/>
       <c r="G31" s="8"/>
       <c r="H31" s="8"/>
-      <c r="I31" s="35"/>
-      <c r="J31" s="35"/>
+      <c r="I31" s="34"/>
+      <c r="J31" s="34"/>
       <c r="K31" s="8"/>
     </row>
   </sheetData>
@@ -1796,125 +1797,125 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="A3" s="18" t="s">
+      <c r="A3" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="B3" s="19" t="s">
+      <c r="B3" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="C3" s="19" t="s">
+      <c r="C3" s="18" t="s">
         <v>41</v>
       </c>
       <c r="D3" s="1"/>
-      <c r="E3" s="18" t="s">
+      <c r="E3" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="F3" s="18" t="s">
+      <c r="F3" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="G3" s="18" t="s">
+      <c r="G3" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="H3" s="18" t="s">
+      <c r="H3" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="I3" s="18" t="s">
+      <c r="I3" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="J3" s="18" t="s">
+      <c r="J3" s="17" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="17" t="s">
+      <c r="A4" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="B4" s="17">
+      <c r="B4" s="16">
         <v>6</v>
       </c>
-      <c r="C4" s="17">
+      <c r="C4" s="16">
         <f t="shared" ref="C4:C9" si="0">B4/30</f>
         <v>0.2</v>
       </c>
-      <c r="E4" s="17">
+      <c r="E4" s="16">
         <v>6</v>
       </c>
-      <c r="F4" s="17">
+      <c r="F4" s="16">
         <v>2</v>
       </c>
-      <c r="G4" s="17">
+      <c r="G4" s="16">
         <f>SUM(E4:F4)</f>
         <v>8</v>
       </c>
-      <c r="H4" s="20">
+      <c r="H4" s="19">
         <f>E4*5</f>
         <v>30</v>
       </c>
-      <c r="I4" s="17">
+      <c r="I4" s="16">
         <f>F4*5</f>
         <v>10</v>
       </c>
-      <c r="J4" s="17">
+      <c r="J4" s="16">
         <f>SUM(H4:I4)</f>
         <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="17" t="s">
+      <c r="A5" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="B5" s="17">
+      <c r="B5" s="16">
         <v>12</v>
       </c>
-      <c r="C5" s="17">
+      <c r="C5" s="16">
         <f t="shared" si="0"/>
         <v>0.4</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="17" t="s">
+      <c r="A6" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="B6" s="17">
+      <c r="B6" s="16">
         <v>18</v>
       </c>
-      <c r="C6" s="17">
+      <c r="C6" s="16">
         <f t="shared" si="0"/>
         <v>0.6</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="17" t="s">
+      <c r="A7" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="B7" s="17">
+      <c r="B7" s="16">
         <v>24</v>
       </c>
-      <c r="C7" s="17">
+      <c r="C7" s="16">
         <f t="shared" si="0"/>
         <v>0.8</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="17" t="s">
+      <c r="A8" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="B8" s="20">
+      <c r="B8" s="19">
         <v>30</v>
       </c>
-      <c r="C8" s="17">
+      <c r="C8" s="16">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="17" t="s">
+      <c r="A9" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="B9" s="17">
+      <c r="B9" s="16">
         <v>60</v>
       </c>
-      <c r="C9" s="17">
+      <c r="C9" s="16">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>

</xml_diff>